<commit_message>
Added players fix (up to 12p) & base prot rework
</commit_message>
<xml_diff>
--- a/Shop minecraft map.xlsx
+++ b/Shop minecraft map.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidatorni\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Games\Nonios's Minigame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D8A351-1CFA-43D1-B7B6-468B8F06BDA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D4F2CC-6F2D-4427-84F4-E3C9D6D97F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7C82B07-5864-4B4F-B7D1-8E1FC637395E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7C82B07-5864-4B4F-B7D1-8E1FC637395E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -947,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35B5616-4B9B-4A24-85D0-2F3EC8F1C901}">
   <dimension ref="B2:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>